<commit_message>
New function. User can choose whether or not pick specific states. It also sends an email in case some clients are unaccessible by the bot. New API error found. Code 403.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahuel.delacruz\OneDrive - Sovos Compliance\Documents\UiPath\SUT_STS_SF_EDIGeneration_ByState\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23B5643-3D4B-49FF-9343-EE62FD3B79A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DD6A8E-22DE-44B4-A5A4-2C436A3CEDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -324,9 +324,6 @@
     <t>Hi team, &lt;br&gt;&lt;br&gt;There was an exception while the bot was running. Here are the details: &lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
-    <t>EDI Generation - Multiple Client</t>
-  </si>
-  <si>
     <t>API_GetStatesList_Endpoint</t>
   </si>
   <si>
@@ -360,15 +357,9 @@
     <t>Request Context</t>
   </si>
   <si>
-    <t>EDI Generation - By States</t>
-  </si>
-  <si>
     <t>Mail_To</t>
   </si>
   <si>
-    <t>Hi team, &lt;br&gt;&lt;br&gt;Here is the status of the bot running "EDI Generation - by States" process. &lt;br&gt;Attached is a zip file with the corresponding EDI files. &lt;br&gt;Here is the status table:</t>
-  </si>
-  <si>
     <t>Mail_HtmlBody_Footer</t>
   </si>
   <si>
@@ -376,6 +367,18 @@
   </si>
   <si>
     <t>Mail_HtmlBody_Header</t>
+  </si>
+  <si>
+    <t>Mail_HtmlBody_ShowFailedClients</t>
+  </si>
+  <si>
+    <t>Hi team, &lt;br&gt;&lt;br&gt;Here is the status of the bot running "EDI Generation - Multiple Clients" process. &lt;br&gt;Attached is a zip file with the corresponding EDI files. &lt;br&gt;Here is the status table:</t>
+  </si>
+  <si>
+    <t>EDI Generation - Multiple Clients</t>
+  </si>
+  <si>
+    <t>Hi team, &lt;br&gt;&lt;br&gt;The bot found some clients with unaccessible data. Here is the list of clients and their details:</t>
   </si>
 </sst>
 </file>
@@ -755,7 +758,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -828,7 +831,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -885,7 +888,7 @@
         <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
         <v>82</v>
@@ -905,18 +908,18 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
         <v>105</v>
-      </c>
-      <c r="B17" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
         <v>102</v>
-      </c>
-      <c r="B18" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
@@ -1922,10 +1925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z970"/>
+  <dimension ref="A1:Z971"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2150,10 +2153,10 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
         <v>96</v>
-      </c>
-      <c r="B25" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2176,18 +2179,18 @@
         <v>72</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
@@ -2241,23 +2244,23 @@
         <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
@@ -2270,23 +2273,33 @@
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>106</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A44" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3213,6 +3226,7 @@
     <row r="968" ht="14.25" customHeight="1"/>
     <row r="969" ht="14.25" customHeight="1"/>
     <row r="970" ht="14.25" customHeight="1"/>
+    <row r="971" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Argument was removed. User can pick only states in the form Legal entity was added in EDI file name and Status table. Bot won't delete the output folder anymore.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahuel.delacruz\OneDrive - Sovos Compliance\Documents\UiPath\SUT_STS_SF_EDIGeneration_ByState\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DD6A8E-22DE-44B4-A5A4-2C436A3CEDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA44027E-7413-49A6-BAEF-BD777AFD886F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="113">
   <si>
     <t>Name</t>
   </si>
@@ -231,15 +231,6 @@
     <t>PathUserOutputFolder</t>
   </si>
   <si>
-    <t>NameEdiXmlFile</t>
-  </si>
-  <si>
-    <t>EDI &lt;RETURN&gt; &lt;ORGANIZATION&gt; &lt;DATETIME&gt;.xml</t>
-  </si>
-  <si>
-    <t>Used in Dispatcher workflow</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -372,13 +363,19 @@
     <t>Mail_HtmlBody_ShowFailedClients</t>
   </si>
   <si>
-    <t>Hi team, &lt;br&gt;&lt;br&gt;Here is the status of the bot running "EDI Generation - Multiple Clients" process. &lt;br&gt;Attached is a zip file with the corresponding EDI files. &lt;br&gt;Here is the status table:</t>
-  </si>
-  <si>
-    <t>EDI Generation - Multiple Clients</t>
-  </si>
-  <si>
     <t>Hi team, &lt;br&gt;&lt;br&gt;The bot found some clients with unaccessible data. Here is the list of clients and their details:</t>
+  </si>
+  <si>
+    <t>StatusTable_LegalEntityColumn</t>
+  </si>
+  <si>
+    <t>Legal Entity</t>
+  </si>
+  <si>
+    <t>EDI Generation - By State</t>
+  </si>
+  <si>
+    <t>Hi team, &lt;br&gt;&lt;br&gt;Here is the status of the bot running "EDI Generation - By State" process. &lt;br&gt;You can find the Output folder here: &lt;b&gt;C:\Users\&lt;USERNAME&gt;\Desktop\EDI Generation output&lt;b&gt; &lt;br&gt;Here is the status table:</t>
   </si>
 </sst>
 </file>
@@ -757,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -805,10 +802,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -819,7 +816,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -831,7 +828,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -843,99 +840,96 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="15" customHeight="1">
+      <c r="A13" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+      <c r="B13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1">
-      <c r="A15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1927,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z971"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2076,26 +2070,26 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2153,10 +2147,10 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2176,21 +2170,21 @@
         <v>49</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
@@ -2241,63 +2235,63 @@
     <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Folders and workflows of Sovos Filing API were replaced by the Sovos Filing API library.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahuel.delacruz\OneDrive - Sovos Compliance\Documents\UiPath\SUT_STS_SF_EDIGeneration_ByState\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA44027E-7413-49A6-BAEF-BD777AFD886F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE4A6ED-7D0C-4790-9FA5-9E5A21B087D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -165,69 +165,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>API_GetOrganizations_Endpoint</t>
-  </si>
-  <si>
-    <t>https://filing.sovos.com/api/v1/iam/users/clients/orgs?root-orgs-only=true</t>
-  </si>
-  <si>
-    <t>API_StandardAppId</t>
-  </si>
-  <si>
-    <t>SUF</t>
-  </si>
-  <si>
-    <t>API_GetReturnsList_Endpoint</t>
-  </si>
-  <si>
-    <t>https://filing.sovos.com/api/v1/returns/returns/&lt;YEAR&gt;/&lt;MONTH&gt;</t>
-  </si>
-  <si>
-    <t>YEAR format = YYYY ; MONTH format = M</t>
-  </si>
-  <si>
-    <t>API_GetReturnsList_Body</t>
-  </si>
-  <si>
-    <t>PathJsonTemplateReturnList</t>
-  </si>
-  <si>
-    <t>Data\JSON Templates\Returns List.txt</t>
-  </si>
-  <si>
-    <t>API_GetEDIXml_Endpoint</t>
-  </si>
-  <si>
-    <t>https://filing.sovos.com/api/v1/returns/filing/render</t>
-  </si>
-  <si>
-    <t>API_GetEDIXml_Body</t>
-  </si>
-  <si>
-    <t>{ "outputType":"FILE", "filingObjectId":&lt;OBJECT_ID&gt;, "validate":false }</t>
-  </si>
-  <si>
-    <t>Replace &lt;OBJECT_ID&gt; with the Return Object ID (obtained from Returns List API)</t>
-  </si>
-  <si>
-    <t>SovosFiling_Cookies_TokenPropertyName</t>
-  </si>
-  <si>
-    <t>token</t>
-  </si>
-  <si>
-    <t>SovosFiling_TokenPrefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bearer </t>
-  </si>
-  <si>
-    <t>This string should be before the token. It will be used with Sovos Filing API</t>
-  </si>
-  <si>
-    <t>Cookie property name to get the token.</t>
-  </si>
-  <si>
     <t>PathUserOutputFolder</t>
   </si>
   <si>
@@ -246,9 +183,6 @@
     <t>The bot finished due to a exception in the initialization phase.</t>
   </si>
   <si>
-    <t>{"filters":[{"by":"FILING_TYPE","type":"IN","value":"EDI","rangeValue":""}]}</t>
-  </si>
-  <si>
     <t>LogMessage_ReturnHasNoInformation</t>
   </si>
   <si>
@@ -315,12 +249,6 @@
     <t>Hi team, &lt;br&gt;&lt;br&gt;There was an exception while the bot was running. Here are the details: &lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
-    <t>API_GetStatesList_Endpoint</t>
-  </si>
-  <si>
-    <t>https://filing.sovos.com/api/v1/filing-metadata/states</t>
-  </si>
-  <si>
     <t>{"filters":[{"by":"FILING_TYPE","type":"IN","value":"EDI","rangeValue":""},{"by":"STATE","type":"IN","value":"&lt;LIST_STATES&gt;","rangeValue":""}]}</t>
   </si>
   <si>
@@ -330,15 +258,9 @@
     <t>API_GetReturnsList_Body_FilterByState</t>
   </si>
   <si>
-    <t>Body to apply filters by ReturnName. Filter returns by Filing Type = EDI.</t>
-  </si>
-  <si>
     <t>StatusTable_ClientColumn</t>
   </si>
   <si>
-    <t>Organization Name</t>
-  </si>
-  <si>
     <t>Status Bot</t>
   </si>
   <si>
@@ -376,6 +298,9 @@
   </si>
   <si>
     <t>Hi team, &lt;br&gt;&lt;br&gt;Here is the status of the bot running "EDI Generation - By State" process. &lt;br&gt;You can find the Output folder here: &lt;b&gt;C:\Users\&lt;USERNAME&gt;\Desktop\EDI Generation output&lt;b&gt; &lt;br&gt;Here is the status table:</t>
+  </si>
+  <si>
+    <t>Client Name</t>
   </si>
 </sst>
 </file>
@@ -752,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -802,10 +727,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -816,7 +741,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -828,7 +753,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -837,101 +762,94 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+    <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="15" customHeight="1">
-      <c r="A13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" t="s">
-        <v>79</v>
+    <row r="12" spans="1:26" ht="15" customHeight="1">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" t="s">
-        <v>84</v>
-      </c>
-    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1908,8 +1826,6 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1919,10 +1835,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z971"/>
+  <dimension ref="A1:Z958"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1972,7 +1888,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>23</v>
@@ -1983,7 +1899,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>39</v>
@@ -2070,26 +1986,26 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2130,174 +2046,96 @@
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
+        <v>72</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="C23" s="2"/>
+    </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>97</v>
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>95</v>
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="C30" s="2"/>
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A35" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B38" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A39" t="s">
-        <v>104</v>
-      </c>
-      <c r="B39" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" t="s">
-        <v>107</v>
-      </c>
-      <c r="B41" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" t="s">
-        <v>103</v>
-      </c>
-      <c r="B42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A44" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -3208,19 +3046,6 @@
     <row r="956" ht="14.25" customHeight="1"/>
     <row r="957" ht="14.25" customHeight="1"/>
     <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>